<commit_message>
Update excel file for tests
</commit_message>
<xml_diff>
--- a/Test/Test.xlsx
+++ b/Test/Test.xlsx
@@ -3,11 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pluto1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pluto" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -17,13 +16,89 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="17">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="True"/>
+    </font>
+    <font>
+      <name val="0"/>
+    </font>
+    <font>
+      <name val="1"/>
+    </font>
+    <font>
+      <i val="1"/>
+    </font>
+    <font>
+      <strike val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="1"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="1"/>
+      <color rgb="000000FF"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="1"/>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="1"/>
+      <color rgb="00FFFF00"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="1"/>
+      <color rgb="0000FFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="00FFFF00"/>
+      <sz val="30"/>
+    </font>
+    <font>
+      <name val="Century Gothic"/>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="00FFFF00"/>
+      <sz val="30"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="00FFFF00"/>
+      <sz val="30"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +121,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -400,7 +490,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
+      <c r="A1" s="15" t="n">
         <v>10</v>
       </c>
     </row>
@@ -410,7 +500,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="15" t="n">
         <v>1000</v>
       </c>
       <c r="G3" t="n">
@@ -429,7 +519,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="D6" t="n">
+      <c r="D6" s="15" t="n">
         <v>76</v>
       </c>
     </row>
@@ -443,22 +533,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring code on excel.py
</commit_message>
<xml_diff>
--- a/Test/Test.xlsx
+++ b/Test/Test.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -95,6 +95,20 @@
     </font>
     <font>
       <name val="Arial"/>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="00FFFF00"/>
+      <sz val="30"/>
+    </font>
+    <font>
+      <name val="MS Comic"/>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="00FFFF00"/>
+      <sz val="30"/>
+    </font>
+    <font>
+      <name val="Comic Sans MS"/>
       <b val="1"/>
       <strike val="0"/>
       <color rgb="00FFFF00"/>
@@ -121,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -138,6 +152,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -490,7 +506,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="n">
+      <c r="A1" s="17" t="n">
         <v>10</v>
       </c>
     </row>
@@ -500,7 +516,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="15" t="n">
+      <c r="A3" s="17" t="n">
         <v>1000</v>
       </c>
       <c r="G3" t="n">
@@ -519,7 +535,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="17" t="n">
         <v>76</v>
       </c>
     </row>

</xml_diff>